<commit_message>
Commit with screenshot implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/TestData.xlsx
+++ b/src/test/resources/excel/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>S.No</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>LN5</t>
+  </si>
+  <si>
+    <t>A1B2Z1</t>
   </si>
 </sst>
 </file>
@@ -405,7 +408,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,7 +499,7 @@
         <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>